<commit_message>
Update misc manufacturing files
</commit_message>
<xml_diff>
--- a/imix_v1_2_oct_2016/imix_cpl.xlsx
+++ b/imix_v1_2_oct_2016/imix_cpl.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Surface Mount" sheetId="1" r:id="rId1"/>
+    <sheet name="Through Hole" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="imix" localSheetId="0">Sheet1!$A$6:$F$142</definedName>
+    <definedName name="imix" localSheetId="0">'Surface Mount'!$A$6:$E$118</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="imix" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/shaneleonard/development/eagle/projects/imix/imix_v1_2_oct_2016/imix.txt" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="/Users/shaneleonard/development/eagle/projects/imix/imix_v1_2_oct_2016/imix.txt" space="1" consecutive="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="133">
   <si>
     <t>Ref Designator</t>
   </si>
@@ -73,9 +74,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>C0603</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -211,39 +209,12 @@
     <t>D9</t>
   </si>
   <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>F3</t>
-  </si>
-  <si>
-    <t>F5</t>
-  </si>
-  <si>
-    <t>F6</t>
-  </si>
-  <si>
-    <t>F7</t>
-  </si>
-  <si>
-    <t>F8</t>
-  </si>
-  <si>
-    <t>F9</t>
-  </si>
-  <si>
-    <t>F10</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
     <t>L2</t>
   </si>
   <si>
-    <t>L1212</t>
-  </si>
-  <si>
     <t>L3</t>
   </si>
   <si>
@@ -259,9 +230,6 @@
     <t>LED5</t>
   </si>
   <si>
-    <t>USER</t>
-  </si>
-  <si>
     <t>Q2</t>
   </si>
   <si>
@@ -295,12 +263,6 @@
     <t>R10</t>
   </si>
   <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
     <t>R13</t>
   </si>
   <si>
@@ -316,9 +278,6 @@
     <t>R17</t>
   </si>
   <si>
-    <t>R18</t>
-  </si>
-  <si>
     <t>R20</t>
   </si>
   <si>
@@ -361,24 +320,6 @@
     <t>R38</t>
   </si>
   <si>
-    <t>RESET</t>
-  </si>
-  <si>
-    <t>SJ6</t>
-  </si>
-  <si>
-    <t>TC1</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>U$1</t>
-  </si>
-  <si>
-    <t>U$4</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -424,9 +365,6 @@
     <t>C7</t>
   </si>
   <si>
-    <t>C45</t>
-  </si>
-  <si>
     <t>C46</t>
   </si>
   <si>
@@ -439,12 +377,6 @@
     <t>C50</t>
   </si>
   <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>F4</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
@@ -457,21 +389,6 @@
     <t>R23</t>
   </si>
   <si>
-    <t>SJ1</t>
-  </si>
-  <si>
-    <t>SJ2</t>
-  </si>
-  <si>
-    <t>SJ3</t>
-  </si>
-  <si>
-    <t>SJ4</t>
-  </si>
-  <si>
-    <t>SJ7</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
@@ -497,6 +414,39 @@
   </si>
   <si>
     <t>Designer: Shane Leonard</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
 </sst>
 </file>
@@ -815,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="86" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -827,25 +777,24 @@
     <col min="2" max="3" width="6.1640625" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -876,7 +825,7 @@
         <v>76.02</v>
       </c>
       <c r="D6" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E6">
         <v>90</v>
@@ -893,7 +842,7 @@
         <v>-3.42</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E7">
         <v>270</v>
@@ -910,7 +859,7 @@
         <v>73.010000000000005</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E8">
         <v>90</v>
@@ -918,7 +867,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>49</v>
@@ -927,7 +876,7 @@
         <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E9">
         <v>270</v>
@@ -935,7 +884,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>51</v>
@@ -944,7 +893,7 @@
         <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E10">
         <v>270</v>
@@ -952,7 +901,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>53</v>
@@ -961,7 +910,7 @@
         <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E11">
         <v>90</v>
@@ -969,7 +918,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>55</v>
@@ -978,7 +927,7 @@
         <v>73</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E12">
         <v>90</v>
@@ -986,7 +935,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>57</v>
@@ -995,7 +944,7 @@
         <v>73</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E13">
         <v>270</v>
@@ -1003,7 +952,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>13.5</v>
@@ -1012,7 +961,7 @@
         <v>48.5</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E14">
         <v>270</v>
@@ -1020,7 +969,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>80</v>
@@ -1029,7 +978,7 @@
         <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1037,7 +986,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>61</v>
@@ -1046,7 +995,7 @@
         <v>68.5</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E16">
         <v>270</v>
@@ -1054,7 +1003,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>45.2</v>
@@ -1063,7 +1012,7 @@
         <v>65.900000000000006</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E17">
         <v>270</v>
@@ -1071,7 +1020,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>12.5</v>
@@ -1080,7 +1029,7 @@
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1088,7 +1037,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>54</v>
@@ -1097,7 +1046,7 @@
         <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1105,7 +1054,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>11</v>
@@ -1114,7 +1063,7 @@
         <v>41.5</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E20">
         <v>180</v>
@@ -1122,7 +1071,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -1131,7 +1080,7 @@
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E21">
         <v>270</v>
@@ -1139,7 +1088,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>13</v>
@@ -1148,7 +1097,7 @@
         <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E22">
         <v>90</v>
@@ -1156,7 +1105,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>43.11</v>
@@ -1165,7 +1114,7 @@
         <v>38.97</v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1173,7 +1122,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>68.25</v>
@@ -1182,7 +1131,7 @@
         <v>37.75</v>
       </c>
       <c r="D24" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E24">
         <v>90</v>
@@ -1190,7 +1139,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>37</v>
@@ -1199,7 +1148,7 @@
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E25">
         <v>225</v>
@@ -1207,7 +1156,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>46.5</v>
@@ -1216,7 +1165,7 @@
         <v>28.5</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E26">
         <v>315</v>
@@ -1224,7 +1173,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>38</v>
@@ -1233,7 +1182,7 @@
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E27">
         <v>315</v>
@@ -1241,7 +1190,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>40.5</v>
@@ -1250,7 +1199,7 @@
         <v>24.5</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E28">
         <v>315</v>
@@ -1258,7 +1207,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>59</v>
@@ -1267,7 +1216,7 @@
         <v>23.5</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E29">
         <v>180</v>
@@ -1275,7 +1224,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>46.75</v>
@@ -1284,7 +1233,7 @@
         <v>22.25</v>
       </c>
       <c r="D30" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E30">
         <v>315</v>
@@ -1292,7 +1241,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>59</v>
@@ -1301,7 +1250,7 @@
         <v>21.5</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E31">
         <v>180</v>
@@ -1309,7 +1258,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>45.25</v>
@@ -1318,15 +1267,15 @@
         <v>20.75</v>
       </c>
       <c r="D32" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E32">
         <v>315</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>80</v>
@@ -1335,15 +1284,15 @@
         <v>27.5</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E33">
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>54</v>
@@ -1352,18 +1301,15 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E34">
         <v>90</v>
       </c>
-      <c r="F34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>67</v>
@@ -1372,18 +1318,15 @@
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>67</v>
@@ -1392,15 +1335,15 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>67</v>
@@ -1409,15 +1352,15 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E37">
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>64</v>
@@ -1426,18 +1369,15 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E38">
         <v>270</v>
       </c>
-      <c r="F38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>53</v>
@@ -1446,18 +1386,15 @@
         <v>-2.5</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E39">
         <v>180</v>
       </c>
-      <c r="F39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>58</v>
@@ -1466,18 +1403,15 @@
         <v>-4.5</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E40">
         <v>270</v>
       </c>
-      <c r="F40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>62.5</v>
@@ -1486,18 +1420,15 @@
         <v>-4.5</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E41">
         <v>270</v>
       </c>
-      <c r="F41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <v>67</v>
@@ -1506,15 +1437,15 @@
         <v>-5.5</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>84</v>
@@ -1523,15 +1454,15 @@
         <v>3.5</v>
       </c>
       <c r="D43" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>84</v>
@@ -1540,15 +1471,15 @@
         <v>1.5</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>84</v>
@@ -1557,15 +1488,15 @@
         <v>-0.5</v>
       </c>
       <c r="D45" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>84</v>
@@ -1574,15 +1505,15 @@
         <v>-2.5</v>
       </c>
       <c r="D46" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>68.12</v>
@@ -1591,15 +1522,15 @@
         <v>71.510000000000005</v>
       </c>
       <c r="D47" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>71.8</v>
@@ -1608,15 +1539,15 @@
         <v>67.05</v>
       </c>
       <c r="D48" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E48">
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49">
         <v>7.86</v>
@@ -1625,15 +1556,15 @@
         <v>37.130000000000003</v>
       </c>
       <c r="D49" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E49">
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>8.36</v>
@@ -1642,15 +1573,15 @@
         <v>23.06</v>
       </c>
       <c r="D50" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E50">
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51">
         <v>80.44</v>
@@ -1659,15 +1590,15 @@
         <v>82.92</v>
       </c>
       <c r="D51" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52">
         <v>83.5</v>
@@ -1676,15 +1607,15 @@
         <v>68</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E52">
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <v>40.65</v>
@@ -1693,214 +1624,211 @@
         <v>11.56</v>
       </c>
       <c r="D53" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>68.849999999999994</v>
+      </c>
+      <c r="C54">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="D54" t="s">
+        <v>116</v>
+      </c>
+      <c r="E54">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B54">
-        <v>2</v>
-      </c>
-      <c r="C54">
+      <c r="B55">
+        <v>49.71</v>
+      </c>
+      <c r="C55">
+        <v>23.6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>79.5</v>
+      </c>
+      <c r="C56">
         <v>68</v>
       </c>
-      <c r="D54" t="s">
-        <v>144</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55">
-        <v>78.5</v>
-      </c>
-      <c r="C55">
-        <v>-14.5</v>
-      </c>
-      <c r="D55" t="s">
-        <v>144</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="D56" t="s">
+        <v>116</v>
+      </c>
+      <c r="E56">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B56">
-        <v>38</v>
-      </c>
-      <c r="C56">
-        <v>46</v>
-      </c>
-      <c r="D56" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <v>44.5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B57">
-        <v>74.5</v>
-      </c>
-      <c r="C57">
-        <v>25.5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>144</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B58">
+        <v>3</v>
+      </c>
+      <c r="C58">
+        <v>41.5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>116</v>
+      </c>
+      <c r="E58">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B58">
-        <v>41</v>
-      </c>
-      <c r="C58">
-        <v>72.5</v>
-      </c>
-      <c r="D58" t="s">
-        <v>144</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B59">
+        <v>52.85</v>
+      </c>
+      <c r="C59">
+        <v>1.38</v>
+      </c>
+      <c r="D59" t="s">
+        <v>116</v>
+      </c>
+      <c r="E59">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B59">
-        <v>61.5</v>
-      </c>
-      <c r="C59">
-        <v>64.5</v>
-      </c>
-      <c r="D59" t="s">
-        <v>144</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B60">
+        <v>84</v>
+      </c>
+      <c r="C60">
+        <v>31.5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>116</v>
+      </c>
+      <c r="E60">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B60">
-        <v>36.5</v>
-      </c>
-      <c r="C60">
-        <v>13.5</v>
-      </c>
-      <c r="D60" t="s">
-        <v>144</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="B61">
+        <v>27.05</v>
+      </c>
+      <c r="C61">
+        <v>26</v>
+      </c>
+      <c r="D61" t="s">
+        <v>116</v>
+      </c>
+      <c r="E61">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B61">
-        <v>73.5</v>
-      </c>
-      <c r="C61">
-        <v>-6.5</v>
-      </c>
-      <c r="D61" t="s">
-        <v>144</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="B62">
+        <v>27.05</v>
+      </c>
+      <c r="C62">
+        <v>22.5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>116</v>
+      </c>
+      <c r="E62">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B62">
-        <v>68.849999999999994</v>
-      </c>
-      <c r="C62">
-        <v>40.799999999999997</v>
-      </c>
-      <c r="D62" t="s">
-        <v>144</v>
-      </c>
-      <c r="E62">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="B63">
+        <v>27.05</v>
+      </c>
+      <c r="C63">
+        <v>19</v>
+      </c>
+      <c r="D63" t="s">
+        <v>116</v>
+      </c>
+      <c r="E63">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B63">
-        <v>49.71</v>
-      </c>
-      <c r="C63">
-        <v>23.6</v>
-      </c>
-      <c r="D63" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63">
-        <v>315</v>
-      </c>
-      <c r="F63" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>65</v>
-      </c>
       <c r="B64">
-        <v>79.5</v>
+        <v>27.05</v>
       </c>
       <c r="C64">
-        <v>68</v>
+        <v>15.5</v>
       </c>
       <c r="D64" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E64">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>26.03</v>
       </c>
       <c r="C65">
-        <v>44.5</v>
+        <v>58.99</v>
       </c>
       <c r="D65" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E65">
         <v>90</v>
@@ -1908,16 +1836,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>27.99</v>
       </c>
       <c r="C66">
-        <v>41.5</v>
+        <v>58.99</v>
       </c>
       <c r="D66" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E66">
         <v>90</v>
@@ -1925,16 +1853,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B67">
-        <v>52.85</v>
+        <v>30</v>
       </c>
       <c r="C67">
-        <v>1.38</v>
+        <v>59</v>
       </c>
       <c r="D67" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E67">
         <v>270</v>
@@ -1942,16 +1870,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B68">
-        <v>84</v>
+        <v>32.1</v>
       </c>
       <c r="C68">
-        <v>31.5</v>
+        <v>21.4</v>
       </c>
       <c r="D68" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E68">
         <v>270</v>
@@ -1959,237 +1887,237 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B69">
-        <v>27.05</v>
+        <v>32</v>
       </c>
       <c r="C69">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D69" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E69">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B70">
-        <v>27.05</v>
+        <v>72.63</v>
       </c>
       <c r="C70">
-        <v>22.5</v>
+        <v>79.5</v>
       </c>
       <c r="D70" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E70">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B71">
-        <v>27.05</v>
+        <v>80</v>
       </c>
       <c r="C71">
-        <v>19</v>
+        <v>80.5</v>
       </c>
       <c r="D71" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E71">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B72">
-        <v>27.05</v>
+        <v>72.599999999999994</v>
       </c>
       <c r="C72">
-        <v>15.5</v>
+        <v>71.5</v>
       </c>
       <c r="D72" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E72">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B73">
-        <v>26.03</v>
+        <v>80</v>
       </c>
       <c r="C73">
-        <v>58.99</v>
+        <v>76.2</v>
       </c>
       <c r="D73" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E73">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B74">
-        <v>27.99</v>
+        <v>83.1</v>
       </c>
       <c r="C74">
-        <v>58.99</v>
+        <v>74.7</v>
       </c>
       <c r="D74" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E74">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B75">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C75">
-        <v>59</v>
+        <v>54.5</v>
       </c>
       <c r="D75" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E75">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B76">
-        <v>32.1</v>
+        <v>12.5</v>
       </c>
       <c r="C76">
-        <v>21.4</v>
+        <v>54.5</v>
       </c>
       <c r="D76" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E76">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B77">
-        <v>32</v>
+        <v>6.5</v>
       </c>
       <c r="C77">
-        <v>27</v>
+        <v>44.5</v>
       </c>
       <c r="D77" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E77">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B78">
-        <v>72.63</v>
+        <v>6.5</v>
       </c>
       <c r="C78">
-        <v>79.5</v>
+        <v>42.5</v>
       </c>
       <c r="D78" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B79">
         <v>80</v>
       </c>
       <c r="C79">
-        <v>80.5</v>
+        <v>31.5</v>
       </c>
       <c r="D79" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E79">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B80">
         <v>80</v>
       </c>
       <c r="C80">
-        <v>78.400000000000006</v>
+        <v>29.5</v>
       </c>
       <c r="D80" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E80">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B81">
-        <v>83</v>
+        <v>44.5</v>
       </c>
       <c r="C81">
-        <v>79.400000000000006</v>
+        <v>24.5</v>
       </c>
       <c r="D81" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E81">
-        <v>270</v>
+        <v>225</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B82">
-        <v>72.599999999999994</v>
+        <v>8.5</v>
       </c>
       <c r="C82">
-        <v>71.5</v>
+        <v>20.5</v>
       </c>
       <c r="D82" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2197,33 +2125,33 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B83">
-        <v>80</v>
+        <v>8.5</v>
       </c>
       <c r="C83">
-        <v>76.2</v>
+        <v>18.5</v>
       </c>
       <c r="D83" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E83">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B84">
-        <v>83.1</v>
+        <v>85</v>
       </c>
       <c r="C84">
-        <v>74.7</v>
+        <v>65.5</v>
       </c>
       <c r="D84" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E84">
         <v>270</v>
@@ -2231,67 +2159,67 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B85">
-        <v>9</v>
+        <v>27.5</v>
       </c>
       <c r="C85">
-        <v>54.5</v>
+        <v>6</v>
       </c>
       <c r="D85" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B86">
-        <v>12.5</v>
+        <v>52</v>
       </c>
       <c r="C86">
-        <v>54.5</v>
+        <v>4</v>
       </c>
       <c r="D86" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B87">
-        <v>7.5</v>
+        <v>53</v>
       </c>
       <c r="C87">
-        <v>49.5</v>
+        <v>-0.5</v>
       </c>
       <c r="D87" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E87">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B88">
-        <v>6.5</v>
+        <v>53</v>
       </c>
       <c r="C88">
-        <v>44.5</v>
+        <v>-4.5</v>
       </c>
       <c r="D88" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E88">
         <v>180</v>
@@ -2299,186 +2227,186 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B89">
-        <v>6.5</v>
+        <v>84</v>
       </c>
       <c r="C89">
-        <v>42.5</v>
+        <v>5.5</v>
       </c>
       <c r="D89" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E89">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B90">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C90">
-        <v>31.5</v>
+        <v>-4.5</v>
       </c>
       <c r="D90" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="B91">
-        <v>80</v>
+        <v>21.82</v>
       </c>
       <c r="C91">
-        <v>29.5</v>
+        <v>6.07</v>
       </c>
       <c r="D91" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>44.5</v>
+        <v>4.5</v>
       </c>
       <c r="C92">
-        <v>24.5</v>
+        <v>53</v>
       </c>
       <c r="D92" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E92">
-        <v>225</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B93">
-        <v>8.5</v>
+        <v>50</v>
       </c>
       <c r="C93">
-        <v>20.5</v>
+        <v>67.569999999999993</v>
       </c>
       <c r="D93" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B94">
-        <v>8.5</v>
+        <v>70.31</v>
       </c>
       <c r="C94">
-        <v>18.5</v>
+        <v>75.31</v>
       </c>
       <c r="D94" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B95">
-        <v>85</v>
+        <v>11.03</v>
       </c>
       <c r="C95">
-        <v>65.5</v>
+        <v>44.91</v>
       </c>
       <c r="D95" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E95">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B96">
-        <v>27.5</v>
+        <v>57</v>
       </c>
       <c r="C96">
-        <v>6</v>
+        <v>35.5</v>
       </c>
       <c r="D96" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E96">
-        <v>270</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B97">
-        <v>52</v>
+        <v>82.23</v>
       </c>
       <c r="C97">
-        <v>4</v>
+        <v>22.51</v>
       </c>
       <c r="D97" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E97">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B98">
-        <v>53</v>
+        <v>59.5</v>
       </c>
       <c r="C98">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E98">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B99">
-        <v>53</v>
+        <v>78.77</v>
       </c>
       <c r="C99">
-        <v>-4.5</v>
+        <v>4.78</v>
       </c>
       <c r="D99" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E99">
         <v>180</v>
@@ -2486,67 +2414,67 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>84</v>
+        <v>76.64</v>
       </c>
       <c r="C100">
-        <v>5.5</v>
+        <v>-1.61</v>
       </c>
       <c r="D100" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>84</v>
+        <v>3.57</v>
       </c>
       <c r="C101">
-        <v>-4.5</v>
+        <v>19.25</v>
       </c>
       <c r="D101" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E101">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B102">
-        <v>21.82</v>
+        <v>3.57</v>
       </c>
       <c r="C102">
-        <v>6.07</v>
+        <v>33.32</v>
       </c>
       <c r="D102" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E102">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B103">
-        <v>79</v>
+        <v>21.82</v>
       </c>
       <c r="C103">
-        <v>65.5</v>
+        <v>64.28</v>
       </c>
       <c r="D103" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E103">
         <v>180</v>
@@ -2554,16 +2482,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B104">
-        <v>44.25</v>
+        <v>57.5</v>
       </c>
       <c r="C104">
-        <v>-3.25</v>
+        <v>68.25</v>
       </c>
       <c r="D104" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E104">
         <v>270</v>
@@ -2571,203 +2499,203 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B105">
-        <v>44.25</v>
+        <v>41.66</v>
       </c>
       <c r="C105">
-        <v>5.75</v>
+        <v>28.14</v>
       </c>
       <c r="D105" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E105">
-        <v>90</v>
+        <v>135</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B106">
-        <v>47.53</v>
+        <v>67.09</v>
       </c>
       <c r="C106">
-        <v>78.64</v>
+        <v>-1.2</v>
       </c>
       <c r="D106" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B107">
-        <v>61.65</v>
+        <v>76</v>
       </c>
       <c r="C107">
-        <v>-8.8800000000000008</v>
+        <v>72</v>
       </c>
       <c r="D107" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E107">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B108">
-        <v>4.5</v>
+        <v>80.5</v>
       </c>
       <c r="C108">
-        <v>53</v>
+        <v>81.5</v>
       </c>
       <c r="D108" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E108">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B109">
-        <v>50</v>
+        <v>84.5</v>
       </c>
       <c r="C109">
-        <v>67.569999999999993</v>
+        <v>69.5</v>
       </c>
       <c r="D109" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E109">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B110">
-        <v>70.31</v>
+        <v>81.5</v>
       </c>
       <c r="C110">
-        <v>75.31</v>
+        <v>70.5</v>
       </c>
       <c r="D110" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E110">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B111">
-        <v>11.03</v>
+        <v>59.25</v>
       </c>
       <c r="C111">
-        <v>44.91</v>
+        <v>37</v>
       </c>
       <c r="D111" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E111">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B112">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="C112">
-        <v>35.5</v>
+        <v>22.8</v>
       </c>
       <c r="D112" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E112">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B113">
-        <v>82.23</v>
+        <v>35.619999999999997</v>
       </c>
       <c r="C113">
-        <v>22.51</v>
+        <v>22.8</v>
       </c>
       <c r="D113" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E113">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B114">
-        <v>59.5</v>
+        <v>7.4</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="D114" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E114">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>112</v>
+      </c>
+      <c r="B115">
+        <v>7.4</v>
+      </c>
+      <c r="C115">
+        <v>30.7</v>
+      </c>
+      <c r="D115" t="s">
         <v>117</v>
       </c>
-      <c r="B115">
-        <v>78.77</v>
-      </c>
-      <c r="C115">
-        <v>4.78</v>
-      </c>
-      <c r="D115" t="s">
-        <v>144</v>
-      </c>
       <c r="E115">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B116">
-        <v>76.64</v>
+        <v>80.14</v>
       </c>
       <c r="C116">
-        <v>-1.61</v>
+        <v>75.150000000000006</v>
       </c>
       <c r="D116" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E116">
         <v>180</v>
@@ -2775,444 +2703,242 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B117">
-        <v>3.57</v>
+        <v>12</v>
       </c>
       <c r="C117">
-        <v>19.25</v>
+        <v>33.5</v>
       </c>
       <c r="D117" t="s">
-        <v>144</v>
+        <v>117</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>115</v>
+      </c>
+      <c r="B118">
+        <v>82</v>
+      </c>
+      <c r="C118">
+        <v>65.5</v>
+      </c>
+      <c r="D118" t="s">
+        <v>117</v>
+      </c>
+      <c r="E118">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>120</v>
       </c>
-      <c r="B118">
-        <v>3.57</v>
-      </c>
-      <c r="C118">
-        <v>33.32</v>
-      </c>
-      <c r="D118" t="s">
-        <v>144</v>
-      </c>
-      <c r="E118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>70</v>
-      </c>
-      <c r="B119">
-        <v>21.82</v>
-      </c>
-      <c r="C119">
-        <v>64.28</v>
-      </c>
-      <c r="D119" t="s">
-        <v>144</v>
-      </c>
-      <c r="E119">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>121</v>
-      </c>
-      <c r="B120">
-        <v>57.5</v>
-      </c>
-      <c r="C120">
-        <v>68.25</v>
-      </c>
-      <c r="D120" t="s">
-        <v>144</v>
-      </c>
-      <c r="E120">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>122</v>
-      </c>
-      <c r="B121">
-        <v>41.66</v>
-      </c>
-      <c r="C121">
-        <v>28.14</v>
-      </c>
-      <c r="D121" t="s">
-        <v>144</v>
-      </c>
-      <c r="E121">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>123</v>
-      </c>
-      <c r="B122">
-        <v>67.09</v>
-      </c>
-      <c r="C122">
-        <v>-1.2</v>
-      </c>
-      <c r="D122" t="s">
-        <v>144</v>
-      </c>
-      <c r="E122">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6">
+        <v>21.6</v>
+      </c>
+      <c r="C6">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7">
+        <v>48.7</v>
+      </c>
+      <c r="C7">
+        <v>58.5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="C8">
+        <v>58.5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9">
+        <v>21.6</v>
+      </c>
+      <c r="C9">
+        <v>20.2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10">
+        <v>55.4</v>
+      </c>
+      <c r="C10">
+        <v>12.8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11">
+        <v>75.7</v>
+      </c>
+      <c r="C11">
+        <v>12.8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12">
+        <v>83.4</v>
+      </c>
+      <c r="C12">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E12">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13">
+        <v>76</v>
+      </c>
+      <c r="C13">
+        <v>79.7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13">
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>124</v>
-      </c>
-      <c r="B123">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14">
         <v>76</v>
       </c>
-      <c r="C123">
-        <v>72</v>
-      </c>
-      <c r="D123" t="s">
-        <v>145</v>
-      </c>
-      <c r="E123">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>125</v>
-      </c>
-      <c r="B124">
-        <v>80.5</v>
-      </c>
-      <c r="C124">
-        <v>83.5</v>
-      </c>
-      <c r="D124" t="s">
-        <v>145</v>
-      </c>
-      <c r="E124">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>126</v>
-      </c>
-      <c r="B125">
-        <v>80.5</v>
-      </c>
-      <c r="C125">
-        <v>81.5</v>
-      </c>
-      <c r="D125" t="s">
-        <v>145</v>
-      </c>
-      <c r="E125">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>127</v>
-      </c>
-      <c r="B126">
-        <v>84.5</v>
-      </c>
-      <c r="C126">
-        <v>69.5</v>
-      </c>
-      <c r="D126" t="s">
-        <v>145</v>
-      </c>
-      <c r="E126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>128</v>
-      </c>
-      <c r="B127">
-        <v>81.5</v>
-      </c>
-      <c r="C127">
-        <v>70.5</v>
-      </c>
-      <c r="D127" t="s">
-        <v>145</v>
-      </c>
-      <c r="E127">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>129</v>
-      </c>
-      <c r="B128">
-        <v>59.25</v>
-      </c>
-      <c r="C128">
-        <v>37</v>
-      </c>
-      <c r="D128" t="s">
-        <v>145</v>
-      </c>
-      <c r="E128">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>130</v>
-      </c>
-      <c r="B129">
-        <v>85</v>
-      </c>
-      <c r="C129">
-        <v>84</v>
-      </c>
-      <c r="D129" t="s">
-        <v>145</v>
-      </c>
-      <c r="E129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>131</v>
-      </c>
-      <c r="B130">
-        <v>2</v>
-      </c>
-      <c r="C130">
-        <v>2</v>
-      </c>
-      <c r="D130" t="s">
-        <v>145</v>
-      </c>
-      <c r="E130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>132</v>
-      </c>
-      <c r="B131">
-        <v>34</v>
-      </c>
-      <c r="C131">
-        <v>22.8</v>
-      </c>
-      <c r="D131" t="s">
-        <v>145</v>
-      </c>
-      <c r="E131">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>133</v>
-      </c>
-      <c r="B132">
-        <v>35.619999999999997</v>
-      </c>
-      <c r="C132">
-        <v>22.8</v>
-      </c>
-      <c r="D132" t="s">
-        <v>145</v>
-      </c>
-      <c r="E132">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>134</v>
-      </c>
-      <c r="B133">
-        <v>7.4</v>
-      </c>
-      <c r="C133">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="D133" t="s">
-        <v>145</v>
-      </c>
-      <c r="E133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>135</v>
-      </c>
-      <c r="B134">
-        <v>7.4</v>
-      </c>
-      <c r="C134">
-        <v>30.7</v>
-      </c>
-      <c r="D134" t="s">
-        <v>145</v>
-      </c>
-      <c r="E134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>136</v>
-      </c>
-      <c r="B135">
-        <v>21.6</v>
-      </c>
-      <c r="C135">
-        <v>17.760000000000002</v>
-      </c>
-      <c r="D135" t="s">
-        <v>145</v>
-      </c>
-      <c r="E135">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>137</v>
-      </c>
-      <c r="B136">
-        <v>21.59</v>
-      </c>
-      <c r="C136">
-        <v>15.24</v>
-      </c>
-      <c r="D136" t="s">
-        <v>145</v>
-      </c>
-      <c r="E136">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>138</v>
-      </c>
-      <c r="B137">
-        <v>21.68</v>
-      </c>
-      <c r="C137">
-        <v>25.39</v>
-      </c>
-      <c r="D137" t="s">
-        <v>145</v>
-      </c>
-      <c r="E137">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>139</v>
-      </c>
-      <c r="B138">
-        <v>21.61</v>
-      </c>
-      <c r="C138">
-        <v>20.32</v>
-      </c>
-      <c r="D138" t="s">
-        <v>145</v>
-      </c>
-      <c r="E138">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>140</v>
-      </c>
-      <c r="B139">
-        <v>21.65</v>
-      </c>
-      <c r="C139">
-        <v>22.85</v>
-      </c>
-      <c r="D139" t="s">
-        <v>145</v>
-      </c>
-      <c r="E139">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>141</v>
-      </c>
-      <c r="B140">
-        <v>80.14</v>
-      </c>
-      <c r="C140">
-        <v>75.150000000000006</v>
-      </c>
-      <c r="D140" t="s">
-        <v>145</v>
-      </c>
-      <c r="E140">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>142</v>
-      </c>
-      <c r="B141">
-        <v>12</v>
-      </c>
-      <c r="C141">
-        <v>33.5</v>
-      </c>
-      <c r="D141" t="s">
-        <v>145</v>
-      </c>
-      <c r="E141">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>143</v>
-      </c>
-      <c r="B142">
-        <v>82</v>
-      </c>
-      <c r="C142">
-        <v>65.5</v>
-      </c>
-      <c r="D142" t="s">
-        <v>145</v>
-      </c>
-      <c r="E142">
-        <v>180</v>
+      <c r="C14">
+        <v>70.8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>